<commit_message>
add MPQ db solution
</commit_message>
<xml_diff>
--- a/MPQ example.xlsx
+++ b/MPQ example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kwang2/Documents/py/pcba_allocation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0948156D-40EA-C745-9F93-31F10683A35E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D1AD3B4-C58B-6742-8102-54C9883CA3ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1060" yWindow="460" windowWidth="27740" windowHeight="17540" xr2:uid="{40BD944E-E837-4843-9797-1C46D144E73F}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
   <si>
     <t>[{datetime.date(2021, 6, 25): (267.0, [('FCZ', 97.0), ('TSP', 32.0), ('FOC', 138.0)])}, {datetime.date(2021, 6, 26): (203.0, [('FCZ', 64.0), ('FOC', 139.0)])}, {datetime.date(2021, 7, 1): (4.0, [('FOC', 4.0)])}, {datetime.date(2021, 7, 2): (25.0, [('FOC', 16.0), ('FCZ', 9.0)])}, {datetime.date(2021, 7, 12): (300.0, [('FCZ', 13.0), ('FOC', 287.0)])}, {datetime.date(2021, 7, 19): (1749.0, [('FOC', 779.0), ('FCZ', 86.0), ('TSP', 316.0)])}, {datetime.date(2021, 8, 2): (800.0, [])}, {datetime.date(2021, 8, 9): (560.0, [])}, {datetime.date(2021, 8, 30): (168.0, [])}, {datetime.date(2021, 10, 4): (800.0, [])}, {datetime.date(2021, 10, 11): (370.0, [])}]</t>
   </si>
@@ -64,13 +64,16 @@
   </si>
   <si>
     <t>FCZ (MPQ: 30)</t>
+  </si>
+  <si>
+    <t>68-101194/ 68-102376</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -83,6 +86,14 @@
       <color rgb="FF000000"/>
       <name val="Menlo"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="4">
@@ -117,7 +128,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -140,6 +151,10 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -458,12 +473,12 @@
   <dimension ref="A1:G17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="200" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="15.1640625" customWidth="1"/>
+    <col min="1" max="1" width="26.1640625" customWidth="1"/>
     <col min="6" max="6" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -477,8 +492,13 @@
         <v>1</v>
       </c>
     </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="A5" s="10" t="s">
         <v>9</v>
       </c>
       <c r="B5" s="6">
@@ -496,12 +516,12 @@
       <c r="F5" s="6">
         <v>44396</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+      <c r="A6" s="10" t="s">
         <v>2</v>
       </c>
       <c r="B6" s="2">
@@ -519,13 +539,13 @@
       <c r="F6" s="2">
         <v>86</v>
       </c>
-      <c r="G6">
+      <c r="G6" s="2">
         <f>SUM(B6:F6)</f>
         <v>269</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+      <c r="A7" s="10" t="s">
         <v>3</v>
       </c>
       <c r="B7" s="7">
@@ -543,7 +563,7 @@
       <c r="F7" s="8">
         <v>89</v>
       </c>
-      <c r="G7">
+      <c r="G7" s="2">
         <f>SUM(B7:F7)</f>
         <v>269</v>
       </c>

</xml_diff>